<commit_message>
fixing errors for nonstandard integration tests
</commit_message>
<xml_diff>
--- a/calculation-engine/engine-tests/engine-it-graph/src/test/resources/standardwithconfig_excel_files/case_1.xlsx
+++ b/calculation-engine/engine-tests/engine-it-graph/src/test/resources/standardwithconfig_excel_files/case_1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\spreadsheet\CalculationEngine\calculation-engine\engine-demo\src\main\resources\excel\Real_life_xml\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\spreadsheet\CalculationEngine\calculation-engine\engine-tests\engine-it-graph\src\test\resources\standardwithconfig_excel_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -119,7 +119,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
-    <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -155,7 +155,7 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -438,8 +438,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -544,11 +544,11 @@
         <v>8000</v>
       </c>
       <c r="E13" s="2">
-        <f>(D13/100)*Tax</f>
+        <f>(D13/100)*C3</f>
         <v>1840</v>
       </c>
       <c r="F13" s="4">
-        <f>Hazard_Coef*(C13-1)*2/3</f>
+        <f>C7*(C13-1)*2/3</f>
         <v>0</v>
       </c>
       <c r="G13" s="1">
@@ -562,7 +562,7 @@
         <v>10000</v>
       </c>
       <c r="J13" s="2">
-        <f>E13+Social_Tribute</f>
+        <f>E13+C5</f>
         <v>1890</v>
       </c>
       <c r="K13" s="4">
@@ -588,11 +588,11 @@
         <v>6000</v>
       </c>
       <c r="E14" s="2">
-        <f>(D14/100)*Tax</f>
+        <f>(D14/100)*C3</f>
         <v>1380</v>
       </c>
       <c r="F14" s="4">
-        <f>Hazard_Coef*(C14-1)*2/3</f>
+        <f>C7*(C14-1)*2/3</f>
         <v>0</v>
       </c>
       <c r="G14" s="1">
@@ -606,7 +606,7 @@
         <v>7680</v>
       </c>
       <c r="J14" s="2">
-        <f>E14+Social_Tribute</f>
+        <f>E14+C5</f>
         <v>1430</v>
       </c>
       <c r="K14" s="4">
@@ -632,11 +632,11 @@
         <v>4500</v>
       </c>
       <c r="E15" s="2">
-        <f>(D15/100)*Tax</f>
+        <f>(D15/100)*C3</f>
         <v>1035</v>
       </c>
       <c r="F15" s="4">
-        <f>Hazard_Coef*(C15-1)*2/3</f>
+        <f>C7*(C15-1)*2/3</f>
         <v>333.33333333333331</v>
       </c>
       <c r="G15" s="1">
@@ -650,7 +650,7 @@
         <v>6273.333333333333</v>
       </c>
       <c r="J15" s="2">
-        <f>E15+Social_Tribute</f>
+        <f>E15+C5</f>
         <v>1085</v>
       </c>
       <c r="K15" s="4">

</xml_diff>